<commit_message>
Final draft of Phase Balancing stuff
</commit_message>
<xml_diff>
--- a/test_data/fixtures.xlsx
+++ b/test_data/fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\Documents\Code Projects\sidekick\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ACFBE8-4D92-4451-A055-BCDCCE13C207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C86EBA0-63B7-484C-848F-BC5451CAF24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B676AC8D-178C-49D1-AB06-1BD2EB3E51D7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B676AC8D-178C-49D1-AB06-1BD2EB3E51D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixtures" sheetId="1" r:id="rId1"/>
@@ -1656,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B3F856-4532-4CE6-9B0F-DD11EBD8C6EC}">
   <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1894,7 +1894,7 @@
         <v>3.5</v>
       </c>
       <c r="C29" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Initial Data Patch Work
</commit_message>
<xml_diff>
--- a/test_data/fixtures.xlsx
+++ b/test_data/fixtures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\Documents\Code Projects\sidekick\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C86EBA0-63B7-484C-848F-BC5451CAF24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E691EC0-A9FD-400D-BA53-3AF6085323F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B676AC8D-178C-49D1-AB06-1BD2EB3E51D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B676AC8D-178C-49D1-AB06-1BD2EB3E51D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixtures" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="79">
   <si>
     <t>Sequence #</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>Red Truss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Universe </t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>
@@ -723,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A3E800-38A2-42C3-B866-B223FB14183A}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,9 +740,10 @@
     <col min="1" max="1" width="15.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -749,8 +756,14 @@
       <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -763,8 +776,14 @@
       <c r="D2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -777,8 +796,14 @@
       <c r="D3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -791,8 +816,14 @@
       <c r="D4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -805,8 +836,14 @@
       <c r="D5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -819,8 +856,14 @@
       <c r="D6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -833,8 +876,14 @@
       <c r="D7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -847,8 +896,14 @@
       <c r="D8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -861,8 +916,14 @@
       <c r="D9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -875,8 +936,14 @@
       <c r="D10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -889,8 +956,14 @@
       <c r="D11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -903,8 +976,14 @@
       <c r="D12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -917,8 +996,14 @@
       <c r="D13" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -931,8 +1016,14 @@
       <c r="D14" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -945,8 +1036,14 @@
       <c r="D15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -959,8 +1056,14 @@
       <c r="D16" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -973,8 +1076,14 @@
       <c r="D17" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -987,8 +1096,14 @@
       <c r="D18" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1001,8 +1116,14 @@
       <c r="D19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1015,8 +1136,14 @@
       <c r="D20" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1029,8 +1156,14 @@
       <c r="D21" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1043,8 +1176,14 @@
       <c r="D22" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1057,8 +1196,14 @@
       <c r="D23" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1071,8 +1216,14 @@
       <c r="D24" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1085,8 +1236,14 @@
       <c r="D25" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1099,8 +1256,14 @@
       <c r="D26" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1113,8 +1276,14 @@
       <c r="D27" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1127,8 +1296,14 @@
       <c r="D28" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1141,8 +1316,14 @@
       <c r="D29" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1155,8 +1336,14 @@
       <c r="D30" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1169,8 +1356,14 @@
       <c r="D31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1183,8 +1376,14 @@
       <c r="D32" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1197,8 +1396,14 @@
       <c r="D33" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1211,8 +1416,14 @@
       <c r="D34" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1225,8 +1436,14 @@
       <c r="D35" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1239,8 +1456,14 @@
       <c r="D36" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1253,8 +1476,14 @@
       <c r="D37" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1267,8 +1496,14 @@
       <c r="D38" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1281,8 +1516,14 @@
       <c r="D39" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1295,8 +1536,14 @@
       <c r="D40" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1309,8 +1556,14 @@
       <c r="D41" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1323,8 +1576,14 @@
       <c r="D42" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1337,8 +1596,14 @@
       <c r="D43" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1351,8 +1616,14 @@
       <c r="D44" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1365,8 +1636,14 @@
       <c r="D45" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1379,8 +1656,14 @@
       <c r="D46" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1393,8 +1676,14 @@
       <c r="D47" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1407,8 +1696,14 @@
       <c r="D48" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1421,8 +1716,14 @@
       <c r="D49" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1435,8 +1736,14 @@
       <c r="D50" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1449,8 +1756,14 @@
       <c r="D51" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1463,8 +1776,14 @@
       <c r="D52" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1477,8 +1796,14 @@
       <c r="D53" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1491,8 +1816,14 @@
       <c r="D54" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1505,8 +1836,14 @@
       <c r="D55" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1519,8 +1856,14 @@
       <c r="D56" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1533,8 +1876,14 @@
       <c r="D57" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1547,8 +1896,14 @@
       <c r="D58" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1561,8 +1916,14 @@
       <c r="D59" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1575,8 +1936,14 @@
       <c r="D60" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1589,8 +1956,14 @@
       <c r="D61" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1603,8 +1976,14 @@
       <c r="D62" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1617,8 +1996,14 @@
       <c r="D63" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1631,8 +2016,14 @@
       <c r="D64" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1644,6 +2035,12 @@
       </c>
       <c r="D65" t="s">
         <v>76</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1656,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B3F856-4532-4CE6-9B0F-DD11EBD8C6EC}">
   <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>